<commit_message>
[update] 2020/10/22 - 1
</commit_message>
<xml_diff>
--- a/data/config/schedule.xlsx
+++ b/data/config/schedule.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\myself\4NumStudio\data\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4NumResearch\data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DEA8FC-8F3B-48CE-B2F5-B6A23C2F9E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="API" sheetId="3" r:id="rId2"/>
+    <sheet name="Architecture" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
   <si>
     <t>bigint</t>
   </si>
@@ -464,11 +466,66 @@
     <t>initDbBySid(String sid)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>|</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>營收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income_last_year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去年營收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yoy</t>
+  </si>
+  <si>
+    <t>年增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accurate</t>
+  </si>
+  <si>
+    <t>累計營收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accurate_last_year</t>
+  </si>
+  <si>
+    <t>去年累計</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accurate_yoy</t>
+  </si>
+  <si>
+    <t>累計年增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -630,7 +687,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,6 +747,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -985,28 +1045,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:20">
@@ -1021,31 +1081,31 @@
       </c>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="F5" s="20" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="J5" s="20" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="J5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22"/>
-      <c r="N5" s="20" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
+      <c r="N5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
-      <c r="R5" s="20" t="s">
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="R5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="S5" s="21"/>
-      <c r="T5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="14" t="s">
@@ -1197,6 +1257,15 @@
       <c r="L9" s="16" t="s">
         <v>68</v>
       </c>
+      <c r="N9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="R9" s="11" t="s">
         <v>97</v>
       </c>
@@ -1235,6 +1304,15 @@
       <c r="L10" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="N10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="3" t="s">
@@ -1262,6 +1340,15 @@
       <c r="L11" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="N11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="12" spans="2:20">
       <c r="B12" s="5" t="s">
@@ -1289,6 +1376,15 @@
       <c r="L12" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="N12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="2:20">
       <c r="F13" s="3" t="s">
@@ -1309,6 +1405,15 @@
       <c r="L13" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="N13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="2:20">
       <c r="F14" s="3" t="s">
@@ -1327,6 +1432,15 @@
       <c r="L14" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="N14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="2:20">
       <c r="F15" s="3" t="s">
@@ -1345,6 +1459,15 @@
       <c r="L15" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="N15" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="16" spans="2:20">
       <c r="F16" s="3" t="s">
@@ -1363,8 +1486,9 @@
       <c r="L16" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="6:12">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="6:15">
       <c r="F17" s="3" t="s">
         <v>53</v>
       </c>
@@ -1381,8 +1505,9 @@
       <c r="L17" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="6:12">
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="6:15">
       <c r="F18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1393,7 +1518,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="6:12">
+    <row r="19" spans="6:15">
       <c r="F19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1404,7 +1529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="6:12">
+    <row r="20" spans="6:15">
       <c r="F20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1415,7 +1540,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="6:12">
+    <row r="21" spans="6:15">
       <c r="F21" s="3"/>
       <c r="G21" s="1" t="s">
         <v>0</v>
@@ -1424,7 +1549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="6:12">
+    <row r="22" spans="6:15">
       <c r="F22" s="5"/>
       <c r="G22" s="2" t="s">
         <v>0</v>
@@ -1448,29 +1573,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C9" sqref="C9:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.77734375" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
@@ -1487,7 +1612,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32.4">
+    <row r="5" spans="1:5" ht="34">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1496,21 +1621,21 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="1:5" ht="32.4">
-      <c r="A9" s="24" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" ht="34">
+      <c r="A9" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -1520,10 +1645,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32.4">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+    <row r="10" spans="1:5" ht="34">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" t="s">
         <v>101</v>
       </c>
@@ -1531,10 +1656,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="32.4">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+    <row r="11" spans="1:5" ht="34">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" t="s">
         <v>103</v>
       </c>
@@ -1543,7 +1668,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="18" t="s">
         <v>108</v>
       </c>
@@ -1580,7 +1705,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="81">
+    <row r="19" spans="1:4" ht="85">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -1591,7 +1716,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32.4">
+    <row r="20" spans="1:4" ht="34">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1600,12 +1725,12 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
@@ -1633,19 +1758,19 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="48.6">
+    <row r="33" spans="1:2" ht="51">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1667,4 +1792,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4482B817-C0D0-43E0-9EF5-C34F895D7FF7}">
+  <dimension ref="E4:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:9">
+      <c r="E4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="5:9">
+      <c r="E5" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9">
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>